<commit_message>
Fixed PCBA Package for JLPCB (https://jlcpcb.com/)
</commit_message>
<xml_diff>
--- a/PCBA-Order_Files_for_JLPCB/FreeDSP_SMD_AB_plus_0v2_BOM1.xlsx
+++ b/PCBA-Order_Files_for_JLPCB/FreeDSP_SMD_AB_plus_0v2_BOM1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HILO/Documents/KICAD_DATA/FreeDSP_SMD_AB_plus_II/PCBA-0v2_Order_Files_for_JLPCB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B57A2347-B070-AD4F-9B33-6B8D591B01E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550F24A4-764F-BE4D-92A2-2E0A55DA71AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19480" yWindow="6360" windowWidth="28980" windowHeight="25760"/>
+    <workbookView xWindow="19480" yWindow="3040" windowWidth="28980" windowHeight="25760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JL PCBA" sheetId="2" r:id="rId1"/>
@@ -45,9 +45,6 @@
     <t>R70,R3,R7,R21,R24,R33,R39,R52,R58,R60,R75,R78,R79</t>
   </si>
   <si>
-    <t>R_0805_HandSoldering</t>
-  </si>
-  <si>
     <t>1k</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
   </si>
   <si>
     <t>C1,C5,C7,C10,C25,C29,C34,C18</t>
-  </si>
-  <si>
-    <t>C_0805_HandSoldering</t>
   </si>
   <si>
     <t>150p</t>
@@ -496,11 +490,19 @@
       <t>）</t>
     </r>
   </si>
+  <si>
+    <t>C_0805</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R_0805</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6">
     <font>
       <sz val="12"/>
@@ -917,11 +919,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -934,16 +936,16 @@
   <sheetData>
     <row r="1" spans="1:256" s="7" customFormat="1">
       <c r="A1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>140</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>142</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -1200,156 +1202,156 @@
     </row>
     <row r="2" spans="1:256">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:256">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:256">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:256">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:256">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:256">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:256">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:256">
       <c r="A9" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:256">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:256">
       <c r="A11" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:256">
       <c r="A12" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:256">
@@ -1363,413 +1365,413 @@
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:256">
       <c r="A14" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:256">
       <c r="A15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:256">
       <c r="A16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="D17" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="D20" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D23" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>